<commit_message>
2017-2-23 MsmqTest project commit
</commit_message>
<xml_diff>
--- a/任务计划.xlsx
+++ b/任务计划.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Unity IOC框架实例</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -54,59 +54,69 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>.net WCF服务实例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.net 消息队列实例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>memercached缓存服务实例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>redis缓存服务实例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mongodb非关系数据库实例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jira conference开源项目管理系统搭建</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git本地版本库服务器搭建</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>构建一套系统</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MVC后台管理登录实例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quartz定时任务框架实例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EFCodeFirstTest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UnityIocTest</t>
+  </si>
+  <si>
+    <t>MVCAuthorizeTest</t>
+  </si>
+  <si>
+    <t>WcfServiceTest</t>
+  </si>
+  <si>
+    <t>已完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>开始</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>.net WCF服务实例</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>.net 消息队列实例</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>memercached缓存服务实例</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>redis缓存服务实例</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mongodb非关系数据库实例</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jira conference开源项目管理系统搭建</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>git本地版本库服务器搭建</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>构建一套系统</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MVC后台管理登录实例</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quartz定时任务框架实例</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>项目</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EFCodeFirstTest</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UnityIocTest</t>
   </si>
 </sst>
 </file>
@@ -522,7 +532,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -545,7 +555,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -565,7 +575,7 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -585,7 +595,7 @@
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -593,13 +603,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1">
         <v>42779</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
+      <c r="D4" s="1">
+        <v>42786</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -615,7 +631,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="C6" s="1">
+        <v>42787</v>
+      </c>
+      <c r="D6" s="1">
+        <v>42788</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -623,7 +651,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C7" s="1">
+        <v>42789</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -631,7 +665,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -639,7 +673,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -647,7 +681,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -655,7 +689,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -663,7 +697,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -671,7 +705,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -679,7 +713,7 @@
         <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2017-3-22 WebAPI Owin OAuth2.0  WebAPIOAuth实例签入
</commit_message>
<xml_diff>
--- a/任务计划.xlsx
+++ b/任务计划.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Working\GitProject\AllTecDemo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Working\AllTecDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Unity IOC框架实例</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Base32Code</t>
+  </si>
+  <si>
+    <t>WebAPIOAuth</t>
   </si>
 </sst>
 </file>
@@ -546,7 +549,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -555,7 +558,7 @@
     <col min="2" max="2" width="36.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -642,8 +645,14 @@
       <c r="C5" s="1">
         <v>42790</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>23</v>
+      <c r="D5" s="1">
+        <v>42816</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -692,6 +701,9 @@
       </c>
       <c r="B8" t="s">
         <v>9</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
2017-4-13 log4net 与 Quartz实例签入
</commit_message>
<xml_diff>
--- a/任务计划.xlsx
+++ b/任务计划.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Unity IOC框架实例</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -137,6 +137,16 @@
   </si>
   <si>
     <t>MemcachedTest</t>
+  </si>
+  <si>
+    <t>Log4net记录日志实例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuartzTest</t>
+  </si>
+  <si>
+    <t>Log4netTest</t>
   </si>
 </sst>
 </file>
@@ -552,7 +562,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -760,6 +770,18 @@
       <c r="B13" t="s">
         <v>16</v>
       </c>
+      <c r="C13" s="1">
+        <v>42835</v>
+      </c>
+      <c r="D13" s="1">
+        <v>42838</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -781,6 +803,26 @@
       </c>
       <c r="F15" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="1">
+        <v>42838</v>
+      </c>
+      <c r="D16" s="1">
+        <v>42838</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>